<commit_message>
Finish cleaning and saving
Next: Get annotations on standard size and save them
</commit_message>
<xml_diff>
--- a/Formal/Projektablaufplan_AnnikaNassal.xlsx
+++ b/Formal/Projektablaufplan_AnnikaNassal.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bb6f4b40ea5d3ac6/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\anni\Documents\GitHub\CoopDFKI\Formal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="114_{AE49F268-4872-4E82-9E0D-06EAF1B1EE81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04C0FE1E-E9F1-4302-BD3E-3D83748EF997}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5D0B7D5A-1844-4071-AA1C-7EED19691A29}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{5D0B7D5A-1844-4071-AA1C-7EED19691A29}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -628,33 +628,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0880E1-9C8E-40A0-B6AA-1B6D01F75FF2}">
   <dimension ref="B2:AH44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="X30" sqref="X30"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="X36" sqref="X36:X39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="5" max="5" width="6.6640625" customWidth="1"/>
-    <col min="6" max="7" width="7.109375" customWidth="1"/>
-    <col min="8" max="8" width="6.6640625" customWidth="1"/>
-    <col min="9" max="9" width="7.33203125" customWidth="1"/>
-    <col min="10" max="10" width="7.109375" customWidth="1"/>
-    <col min="11" max="14" width="6.6640625" customWidth="1"/>
-    <col min="15" max="15" width="7.109375" customWidth="1"/>
-    <col min="16" max="18" width="6.6640625" customWidth="1"/>
-    <col min="19" max="19" width="7.5546875" customWidth="1"/>
-    <col min="20" max="26" width="6.6640625" customWidth="1"/>
-    <col min="27" max="27" width="7.88671875" customWidth="1"/>
-    <col min="28" max="34" width="6.6640625" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" customWidth="1"/>
+    <col min="6" max="7" width="7.140625" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" customWidth="1"/>
+    <col min="11" max="14" width="6.7109375" customWidth="1"/>
+    <col min="15" max="15" width="7.140625" customWidth="1"/>
+    <col min="16" max="18" width="6.7109375" customWidth="1"/>
+    <col min="19" max="19" width="7.5703125" customWidth="1"/>
+    <col min="20" max="26" width="6.7109375" customWidth="1"/>
+    <col min="27" max="27" width="7.85546875" customWidth="1"/>
+    <col min="28" max="34" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:34" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:34" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:34" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -668,7 +668,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:34" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -682,7 +682,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:34" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -690,7 +690,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:34" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>9</v>
       </c>
@@ -698,7 +698,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:34" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>12</v>
       </c>
@@ -706,7 +706,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="2:34" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:34" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>51</v>
       </c>
@@ -750,7 +750,7 @@
         <v>43983</v>
       </c>
     </row>
-    <row r="13" spans="2:34" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:34" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>15</v>
       </c>
@@ -827,7 +827,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="2:34" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:34" ht="60" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
         <v>20</v>
       </c>
@@ -867,7 +867,7 @@
       <c r="AG15" s="6"/>
       <c r="AH15" s="6"/>
     </row>
-    <row r="16" spans="2:34" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:34" ht="105" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
         <v>21</v>
       </c>
@@ -907,7 +907,7 @@
       <c r="AG16" s="6"/>
       <c r="AH16" s="6"/>
     </row>
-    <row r="17" spans="2:34" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:34" ht="90" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
         <v>22</v>
       </c>
@@ -953,7 +953,7 @@
       <c r="AG17" s="6"/>
       <c r="AH17" s="6"/>
     </row>
-    <row r="18" spans="2:34" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:34" ht="60" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
         <v>23</v>
       </c>
@@ -991,7 +991,7 @@
       <c r="AG18" s="6"/>
       <c r="AH18" s="6"/>
     </row>
-    <row r="19" spans="2:34" ht="72" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:34" ht="75" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
         <v>24</v>
       </c>
@@ -1033,7 +1033,7 @@
       <c r="AG19" s="6"/>
       <c r="AH19" s="6"/>
     </row>
-    <row r="20" spans="2:34" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:34" ht="60" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
         <v>25</v>
       </c>
@@ -1075,7 +1075,7 @@
       <c r="AG20" s="6"/>
       <c r="AH20" s="6"/>
     </row>
-    <row r="21" spans="2:34" ht="79.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:34" ht="96" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
         <v>26</v>
       </c>
@@ -1118,7 +1118,7 @@
       <c r="AG21" s="6"/>
       <c r="AH21" s="6"/>
     </row>
-    <row r="22" spans="2:34" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:34" ht="75" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="s">
         <v>28</v>
       </c>
@@ -1158,7 +1158,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
     </row>
-    <row r="23" spans="2:34" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:34" ht="45" x14ac:dyDescent="0.25">
       <c r="B23" s="9" t="s">
         <v>35</v>
       </c>
@@ -1198,7 +1198,7 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
     </row>
-    <row r="24" spans="2:34" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:34" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
         <v>45</v>
       </c>
@@ -1238,7 +1238,7 @@
       <c r="AG24" s="6"/>
       <c r="AH24" s="6"/>
     </row>
-    <row r="25" spans="2:34" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:34" ht="120" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
         <v>39</v>
       </c>
@@ -1274,7 +1274,7 @@
       <c r="AG25" s="6"/>
       <c r="AH25" s="6"/>
     </row>
-    <row r="26" spans="2:34" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
         <v>29</v>
       </c>
@@ -1314,8 +1314,8 @@
       <c r="AG26" s="6"/>
       <c r="AH26" s="6"/>
     </row>
-    <row r="27" spans="2:34" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B27" s="9" t="s">
+    <row r="27" spans="2:34" ht="30" x14ac:dyDescent="0.25">
+      <c r="B27" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D27" s="6"/>
@@ -1334,10 +1334,10 @@
       <c r="Q27" s="6"/>
       <c r="R27" s="6"/>
       <c r="S27" s="6"/>
-      <c r="T27" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="U27" s="11" t="s">
+      <c r="T27" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="U27" s="7" t="s">
         <v>27</v>
       </c>
       <c r="V27" s="6"/>
@@ -1354,8 +1354,8 @@
       <c r="AG27" s="6"/>
       <c r="AH27" s="6"/>
     </row>
-    <row r="28" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B28" s="9" t="s">
+    <row r="28" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B28" s="8" t="s">
         <v>30</v>
       </c>
       <c r="D28" s="6"/>
@@ -1374,10 +1374,10 @@
       <c r="Q28" s="6"/>
       <c r="R28" s="6"/>
       <c r="S28" s="6"/>
-      <c r="T28" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="U28" s="11" t="s">
+      <c r="T28" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="U28" s="7" t="s">
         <v>27</v>
       </c>
       <c r="V28" s="6"/>
@@ -1394,8 +1394,8 @@
       <c r="AG28" s="6"/>
       <c r="AH28" s="6"/>
     </row>
-    <row r="29" spans="2:34" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B29" s="9" t="s">
+    <row r="29" spans="2:34" ht="30" x14ac:dyDescent="0.25">
+      <c r="B29" s="8" t="s">
         <v>31</v>
       </c>
       <c r="D29" s="6"/>
@@ -1414,10 +1414,10 @@
       <c r="Q29" s="6"/>
       <c r="R29" s="6"/>
       <c r="S29" s="6"/>
-      <c r="T29" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="U29" s="11" t="s">
+      <c r="T29" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="U29" s="7" t="s">
         <v>27</v>
       </c>
       <c r="V29" s="6"/>
@@ -1434,8 +1434,8 @@
       <c r="AG29" s="6"/>
       <c r="AH29" s="6"/>
     </row>
-    <row r="30" spans="2:34" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="B30" s="9" t="s">
+    <row r="30" spans="2:34" ht="180" x14ac:dyDescent="0.25">
+      <c r="B30" s="8" t="s">
         <v>32</v>
       </c>
       <c r="D30" s="6"/>
@@ -1455,10 +1455,10 @@
       <c r="R30" s="6"/>
       <c r="S30" s="6"/>
       <c r="T30" s="6"/>
-      <c r="U30" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="V30" s="11" t="s">
+      <c r="U30" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="V30" s="7" t="s">
         <v>27</v>
       </c>
       <c r="W30" s="6"/>
@@ -1474,7 +1474,7 @@
       <c r="AG30" s="6"/>
       <c r="AH30" s="6"/>
     </row>
-    <row r="31" spans="2:34" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:34" ht="45" x14ac:dyDescent="0.25">
       <c r="B31" s="9" t="s">
         <v>36</v>
       </c>
@@ -1514,7 +1514,7 @@
       <c r="AG31" s="6"/>
       <c r="AH31" s="6"/>
     </row>
-    <row r="32" spans="2:34" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B32" s="10" t="s">
         <v>33</v>
       </c>
@@ -1554,7 +1554,7 @@
       <c r="AG32" s="6"/>
       <c r="AH32" s="6"/>
     </row>
-    <row r="33" spans="2:34" ht="72" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:34" ht="75" x14ac:dyDescent="0.25">
       <c r="B33" s="10" t="s">
         <v>37</v>
       </c>
@@ -1590,7 +1590,7 @@
       <c r="AG33" s="6"/>
       <c r="AH33" s="6"/>
     </row>
-    <row r="34" spans="2:34" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:34" ht="45" x14ac:dyDescent="0.25">
       <c r="B34" s="10" t="s">
         <v>38</v>
       </c>
@@ -1626,7 +1626,7 @@
       <c r="AG34" s="6"/>
       <c r="AH34" s="6"/>
     </row>
-    <row r="35" spans="2:34" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B35" s="10" t="s">
         <v>34</v>
       </c>
@@ -1664,7 +1664,7 @@
       <c r="AG35" s="6"/>
       <c r="AH35" s="6"/>
     </row>
-    <row r="36" spans="2:34" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:34" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="10" t="s">
         <v>47</v>
       </c>
@@ -1704,7 +1704,7 @@
       <c r="AG36" s="6"/>
       <c r="AH36" s="6"/>
     </row>
-    <row r="37" spans="2:34" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:34" ht="45" x14ac:dyDescent="0.25">
       <c r="B37" s="10" t="s">
         <v>42</v>
       </c>
@@ -1744,7 +1744,7 @@
       <c r="AG37" s="6"/>
       <c r="AH37" s="6"/>
     </row>
-    <row r="38" spans="2:34" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B38" s="10" t="s">
         <v>43</v>
       </c>
@@ -1784,7 +1784,7 @@
       <c r="AG38" s="6"/>
       <c r="AH38" s="6"/>
     </row>
-    <row r="39" spans="2:34" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:34" ht="45" x14ac:dyDescent="0.25">
       <c r="B39" s="10" t="s">
         <v>44</v>
       </c>
@@ -1824,7 +1824,7 @@
       <c r="AG39" s="6"/>
       <c r="AH39" s="6"/>
     </row>
-    <row r="40" spans="2:34" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:34" ht="45" x14ac:dyDescent="0.25">
       <c r="B40" s="10" t="s">
         <v>41</v>
       </c>
@@ -1864,7 +1864,7 @@
       <c r="AG40" s="6"/>
       <c r="AH40" s="6"/>
     </row>
-    <row r="41" spans="2:34" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:34" ht="75" x14ac:dyDescent="0.25">
       <c r="B41" s="10" t="s">
         <v>49</v>
       </c>
@@ -1904,7 +1904,7 @@
       <c r="AG41" s="6"/>
       <c r="AH41" s="6"/>
     </row>
-    <row r="42" spans="2:34" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:34" ht="60" x14ac:dyDescent="0.25">
       <c r="B42" s="10" t="s">
         <v>48</v>
       </c>
@@ -1945,7 +1945,7 @@
       <c r="AG42" s="6"/>
       <c r="AH42" s="6"/>
     </row>
-    <row r="43" spans="2:34" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:34" ht="75" x14ac:dyDescent="0.25">
       <c r="B43" s="10" t="s">
         <v>40</v>
       </c>
@@ -1986,7 +1986,7 @@
       <c r="AG43" s="6"/>
       <c r="AH43" s="6"/>
     </row>
-    <row r="44" spans="2:34" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:34" ht="30" x14ac:dyDescent="0.25">
       <c r="B44" s="9" t="s">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
Finished training data prep
</commit_message>
<xml_diff>
--- a/Formal/Projektablaufplan_AnnikaNassal.xlsx
+++ b/Formal/Projektablaufplan_AnnikaNassal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\annika\Documents\GitHub\CoopDFKI\Formal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE4E73D-9815-4EF6-891B-E1AF62EDA64A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB6A8BC-CAF0-4315-B845-275CE3BD23AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5D0B7D5A-1844-4071-AA1C-7EED19691A29}"/>
   </bookViews>
@@ -280,7 +280,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -305,9 +305,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -628,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0880E1-9C8E-40A0-B6AA-1B6D01F75FF2}">
   <dimension ref="B2:AH44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Y28" sqref="Y1:Y1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1158,8 +1155,8 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
     </row>
-    <row r="23" spans="2:34" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B23" s="9" t="s">
+    <row r="23" spans="2:34" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="8" t="s">
         <v>35</v>
       </c>
       <c r="D23" s="6"/>
@@ -1177,10 +1174,10 @@
       <c r="P23" s="6"/>
       <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
-      <c r="S23" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="T23" s="11" t="s">
+      <c r="S23" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="T23" s="7" t="s">
         <v>27</v>
       </c>
       <c r="U23" s="6"/>
@@ -1475,7 +1472,7 @@
       <c r="AH30" s="6"/>
     </row>
     <row r="31" spans="2:34" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="8" t="s">
         <v>36</v>
       </c>
       <c r="D31" s="6"/>
@@ -1495,10 +1492,10 @@
       <c r="R31" s="6"/>
       <c r="S31" s="6"/>
       <c r="T31" s="6"/>
-      <c r="U31" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="V31" s="11" t="s">
+      <c r="U31" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="V31" s="8" t="s">
         <v>27</v>
       </c>
       <c r="W31" s="6"/>
@@ -1515,7 +1512,7 @@
       <c r="AH31" s="6"/>
     </row>
     <row r="32" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="9" t="s">
         <v>33</v>
       </c>
       <c r="D32" s="6"/>
@@ -1536,10 +1533,10 @@
       <c r="S32" s="6"/>
       <c r="T32" s="6"/>
       <c r="U32" s="6"/>
-      <c r="V32" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="W32" s="6" t="s">
+      <c r="V32" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="W32" s="9" t="s">
         <v>27</v>
       </c>
       <c r="X32" s="6"/>
@@ -1555,7 +1552,7 @@
       <c r="AH32" s="6"/>
     </row>
     <row r="33" spans="2:34" ht="72" x14ac:dyDescent="0.3">
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D33" s="6"/>
@@ -1591,7 +1588,7 @@
       <c r="AH33" s="6"/>
     </row>
     <row r="34" spans="2:34" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D34" s="6"/>
@@ -1627,7 +1624,7 @@
       <c r="AH34" s="6"/>
     </row>
     <row r="35" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="9" t="s">
         <v>34</v>
       </c>
       <c r="D35" s="6"/>
@@ -1649,7 +1646,7 @@
       <c r="T35" s="6"/>
       <c r="U35" s="6"/>
       <c r="V35" s="6"/>
-      <c r="W35" s="6" t="s">
+      <c r="W35" s="9" t="s">
         <v>27</v>
       </c>
       <c r="X35" s="6"/>

</xml_diff>

<commit_message>
Finished preprocessing training data
</commit_message>
<xml_diff>
--- a/Formal/Projektablaufplan_AnnikaNassal.xlsx
+++ b/Formal/Projektablaufplan_AnnikaNassal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\annika\Documents\GitHub\CoopDFKI\Formal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB6A8BC-CAF0-4315-B845-275CE3BD23AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20604CF6-68E7-47CD-A685-9C94563464CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5D0B7D5A-1844-4071-AA1C-7EED19691A29}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="54">
   <si>
     <t>Projektplan</t>
   </si>
@@ -192,6 +192,9 @@
   </si>
   <si>
     <t>Nicht von links und oben abschneiden, da Annotationskoordinaten sonst falsch</t>
+  </si>
+  <si>
+    <t>Validierungsdatensatz</t>
   </si>
 </sst>
 </file>
@@ -623,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0880E1-9C8E-40A0-B6AA-1B6D01F75FF2}">
-  <dimension ref="B2:AH44"/>
+  <dimension ref="B2:AH45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1661,9 +1664,9 @@
       <c r="AG35" s="6"/>
       <c r="AH35" s="6"/>
     </row>
-    <row r="36" spans="2:34" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B36" s="10" t="s">
-        <v>47</v>
+    <row r="36" spans="2:34" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B36" s="9" t="s">
+        <v>53</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
@@ -1684,13 +1687,9 @@
       <c r="T36" s="6"/>
       <c r="U36" s="6"/>
       <c r="V36" s="6"/>
-      <c r="W36" s="6"/>
-      <c r="X36" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y36" s="6" t="s">
-        <v>27</v>
-      </c>
+      <c r="W36" s="9"/>
+      <c r="X36" s="6"/>
+      <c r="Y36" s="6"/>
       <c r="Z36" s="6"/>
       <c r="AA36" s="6"/>
       <c r="AB36" s="6"/>
@@ -1703,7 +1702,7 @@
     </row>
     <row r="37" spans="2:34" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B37" s="10" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
@@ -1741,9 +1740,9 @@
       <c r="AG37" s="6"/>
       <c r="AH37" s="6"/>
     </row>
-    <row r="38" spans="2:34" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:34" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B38" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
@@ -1781,9 +1780,9 @@
       <c r="AG38" s="6"/>
       <c r="AH38" s="6"/>
     </row>
-    <row r="39" spans="2:34" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B39" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
@@ -1823,7 +1822,7 @@
     </row>
     <row r="40" spans="2:34" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B40" s="10" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
@@ -1845,14 +1844,14 @@
       <c r="U40" s="6"/>
       <c r="V40" s="6"/>
       <c r="W40" s="6"/>
-      <c r="X40" s="6"/>
-      <c r="Y40" s="6"/>
-      <c r="Z40" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA40" s="6" t="s">
-        <v>27</v>
-      </c>
+      <c r="X40" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y40" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z40" s="6"/>
+      <c r="AA40" s="6"/>
       <c r="AB40" s="6"/>
       <c r="AC40" s="6"/>
       <c r="AD40" s="6"/>
@@ -1861,9 +1860,9 @@
       <c r="AG40" s="6"/>
       <c r="AH40" s="6"/>
     </row>
-    <row r="41" spans="2:34" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:34" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B41" s="10" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
@@ -1887,13 +1886,13 @@
       <c r="W41" s="6"/>
       <c r="X41" s="6"/>
       <c r="Y41" s="6"/>
-      <c r="Z41" s="6"/>
+      <c r="Z41" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="AA41" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="AB41" s="6" t="s">
-        <v>27</v>
-      </c>
+      <c r="AB41" s="6"/>
       <c r="AC41" s="6"/>
       <c r="AD41" s="6"/>
       <c r="AE41" s="6"/>
@@ -1901,11 +1900,10 @@
       <c r="AG41" s="6"/>
       <c r="AH41" s="6"/>
     </row>
-    <row r="42" spans="2:34" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:34" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B42" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C42" s="6"/>
+        <v>49</v>
+      </c>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
@@ -1929,13 +1927,13 @@
       <c r="X42" s="6"/>
       <c r="Y42" s="6"/>
       <c r="Z42" s="6"/>
-      <c r="AA42" s="6"/>
+      <c r="AA42" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="AB42" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="AC42" s="6" t="s">
-        <v>27</v>
-      </c>
+      <c r="AC42" s="6"/>
       <c r="AD42" s="6"/>
       <c r="AE42" s="6"/>
       <c r="AF42" s="6"/>
@@ -1944,7 +1942,7 @@
     </row>
     <row r="43" spans="2:34" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B43" s="10" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
@@ -1971,21 +1969,21 @@
       <c r="Y43" s="6"/>
       <c r="Z43" s="6"/>
       <c r="AA43" s="6"/>
-      <c r="AB43" s="6"/>
+      <c r="AB43" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="AC43" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="AD43" s="6" t="s">
-        <v>27</v>
-      </c>
+      <c r="AD43" s="6"/>
       <c r="AE43" s="6"/>
       <c r="AF43" s="6"/>
       <c r="AG43" s="6"/>
       <c r="AH43" s="6"/>
     </row>
-    <row r="44" spans="2:34" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B44" s="9" t="s">
-        <v>50</v>
+    <row r="44" spans="2:34" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B44" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
@@ -2004,49 +2002,90 @@
       <c r="Q44" s="6"/>
       <c r="R44" s="6"/>
       <c r="S44" s="6"/>
-      <c r="T44" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="U44" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="V44" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="W44" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="X44" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y44" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z44" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA44" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB44" s="6" t="s">
-        <v>27</v>
-      </c>
+      <c r="T44" s="6"/>
+      <c r="U44" s="6"/>
+      <c r="V44" s="6"/>
+      <c r="W44" s="6"/>
+      <c r="X44" s="6"/>
+      <c r="Y44" s="6"/>
+      <c r="Z44" s="6"/>
+      <c r="AA44" s="6"/>
+      <c r="AB44" s="6"/>
       <c r="AC44" s="6" t="s">
         <v>27</v>
       </c>
       <c r="AD44" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="AE44" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="AF44" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="AG44" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="AH44" s="6" t="s">
+      <c r="AE44" s="6"/>
+      <c r="AF44" s="6"/>
+      <c r="AG44" s="6"/>
+      <c r="AH44" s="6"/>
+    </row>
+    <row r="45" spans="2:34" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B45" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="6"/>
+      <c r="K45" s="6"/>
+      <c r="L45" s="6"/>
+      <c r="M45" s="6"/>
+      <c r="N45" s="6"/>
+      <c r="O45" s="6"/>
+      <c r="P45" s="6"/>
+      <c r="Q45" s="6"/>
+      <c r="R45" s="6"/>
+      <c r="S45" s="6"/>
+      <c r="T45" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="U45" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="V45" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="W45" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="X45" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y45" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z45" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA45" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB45" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC45" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD45" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE45" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF45" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG45" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH45" s="6" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Info about how to fix metrics
</commit_message>
<xml_diff>
--- a/Formal/Projektablaufplan_AnnikaNassal.xlsx
+++ b/Formal/Projektablaufplan_AnnikaNassal.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\annika\Documents\GitHub\CoopDFKI\Formal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4AE14F7-B01D-4120-9B72-2939F4979B74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B0D437-900E-4BC2-B508-52A28BC0F5A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5D0B7D5A-1844-4071-AA1C-7EED19691A29}"/>
   </bookViews>
@@ -628,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0880E1-9C8E-40A0-B6AA-1B6D01F75FF2}">
   <dimension ref="B2:AH45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1665,7 +1665,7 @@
       <c r="AH35" s="6"/>
     </row>
     <row r="36" spans="2:34" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="8" t="s">
         <v>53</v>
       </c>
       <c r="D36" s="6"/>
@@ -1703,7 +1703,7 @@
       <c r="AH36" s="6"/>
     </row>
     <row r="37" spans="2:34" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="8" t="s">
         <v>47</v>
       </c>
       <c r="D37" s="6"/>
@@ -1743,7 +1743,7 @@
       <c r="AH37" s="6"/>
     </row>
     <row r="38" spans="2:34" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="8" t="s">
         <v>42</v>
       </c>
       <c r="D38" s="6"/>
@@ -1783,7 +1783,7 @@
       <c r="AH38" s="6"/>
     </row>
     <row r="39" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="8" t="s">
         <v>43</v>
       </c>
       <c r="D39" s="6"/>
@@ -1823,7 +1823,7 @@
       <c r="AH39" s="6"/>
     </row>
     <row r="40" spans="2:34" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D40" s="6"/>

</xml_diff>